<commit_message>
Made a better loop to prepare lipid data for comparison
</commit_message>
<xml_diff>
--- a/krillINFO.xlsx
+++ b/krillINFO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6bc14b3081350469/Old/placement/alfred-wegener/Bettina Meyer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_D598957AC3574A6C9F312C6A3CA8BD1E25A35029" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22D6A713-A180-4C62-987F-E9ECF56CA489}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_DC04F472C3574A6C9F312C787CAEB07825A3D0D9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFEC99F2-C1ED-4268-96EC-7B53754E4EA8}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>yr</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>recruitment</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -387,10 +384,13 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.73046875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -408,10 +408,10 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>34.085641791044779</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+        <v>17.041290322580643</v>
+      </c>
+      <c r="C2">
+        <v>0.83840000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -419,10 +419,10 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>35.465877551020405</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.64300000000000002</v>
+        <v>0.87959999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -430,10 +430,10 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>22.428261589403974</v>
+        <v>5.6309756097560975</v>
       </c>
       <c r="C4">
-        <v>0.83840000000000003</v>
+        <v>0.74650000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -441,10 +441,10 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>18.587334035656401</v>
+        <v>12.558092105263157</v>
       </c>
       <c r="C5">
-        <v>0.87959999999999994</v>
+        <v>0.4955</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -452,10 +452,10 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>30.425801332758621</v>
+        <v>11.038570620938627</v>
       </c>
       <c r="C6">
-        <v>0.74650000000000005</v>
+        <v>0.41660000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -463,10 +463,10 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>28.783474818780888</v>
+        <v>8.9742483660130716</v>
       </c>
       <c r="C7">
-        <v>0.4955</v>
+        <v>0.30133333333333329</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -474,10 +474,10 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>26.604689526184536</v>
+        <v>2.986470588235294</v>
       </c>
       <c r="C8">
-        <v>0.41660000000000003</v>
+        <v>0.70124999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -485,10 +485,10 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>30.996015184801049</v>
+        <v>7.3007031914624276</v>
       </c>
       <c r="C9">
-        <v>0.30133333333333329</v>
+        <v>0.25166666666666665</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -496,10 +496,10 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>29.076755795183512</v>
+        <v>17.456099290780141</v>
       </c>
       <c r="C10">
-        <v>0.70124999999999993</v>
+        <v>0.69133333333333324</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -507,10 +507,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>34.130735459045056</v>
-      </c>
-      <c r="C11">
-        <v>0.25166666666666665</v>
+        <v>30.863691189496603</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -518,10 +515,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>30.769292225145488</v>
-      </c>
-      <c r="C12">
-        <v>0.69133333333333324</v>
+        <v>17.204920088467741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>